<commit_message>
Began to store varied parameter data
</commit_message>
<xml_diff>
--- a/Varied Parameters.xlsx
+++ b/Varied Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saividyud/Documents/GitHub/NASA_25-26_Rocket_Simulations/ORLab Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saividyud/Documents/GitHub/NASA_25-26_Rocket_Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E094642-61DE-CB44-A6CC-6C24BE42A22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D90263-9D57-8342-9FD2-7873382FB059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{D72F03AF-D0CB-7048-A263-60968BD6DCA1}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{D72F03AF-D0CB-7048-A263-60968BD6DCA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Fin Shape</t>
   </si>
   <si>
-    <t>Fin Angle</t>
-  </si>
-  <si>
     <t>Nose Cone Length</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Air Pressure</t>
   </si>
   <si>
-    <t>Fin Thickness</t>
-  </si>
-  <si>
     <t>setGeodeticComputation</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Constant</t>
   </si>
   <si>
-    <t>Trapezoidal, Elliptical</t>
-  </si>
-  <si>
     <t>[286, 302] K</t>
   </si>
   <si>
@@ -201,12 +192,6 @@
     <t>[0, 360) deg</t>
   </si>
   <si>
-    <t>0.137 in</t>
-  </si>
-  <si>
-    <t>0 deg</t>
-  </si>
-  <si>
     <t>Function Name</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
     <t>28.5 in</t>
   </si>
   <si>
-    <t>0.125 in</t>
-  </si>
-  <si>
     <t>6.125 in</t>
   </si>
   <si>
@@ -238,6 +220,36 @@
   </si>
   <si>
     <t>26 in</t>
+  </si>
+  <si>
+    <t>{Trapezoidal, Elliptical, Parallelogram, Swept Trapezoidal}</t>
+  </si>
+  <si>
+    <t>34 in</t>
+  </si>
+  <si>
+    <t>42 in</t>
+  </si>
+  <si>
+    <t>0.1 in</t>
+  </si>
+  <si>
+    <t>0.01 in</t>
+  </si>
+  <si>
+    <t>2.2 lbs</t>
+  </si>
+  <si>
+    <t>0.01 lbs</t>
+  </si>
+  <si>
+    <t>2.7 lbs</t>
+  </si>
+  <si>
+    <t>1.9 lbs</t>
+  </si>
+  <si>
+    <t>3.4 lbs</t>
   </si>
 </sst>
 </file>
@@ -335,10 +347,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D43AC392-C9D8-814D-AE4E-23CC2E89DE4B}" name="Table2" displayName="Table2" ref="A1:F42" totalsRowShown="0">
-  <autoFilter ref="A1:F42" xr:uid="{D43AC392-C9D8-814D-AE4E-23CC2E89DE4B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
-    <sortCondition ref="B1:B42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D43AC392-C9D8-814D-AE4E-23CC2E89DE4B}" name="Table2" displayName="Table2" ref="A1:F40" totalsRowShown="0">
+  <autoFilter ref="A1:F40" xr:uid="{D43AC392-C9D8-814D-AE4E-23CC2E89DE4B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
+    <sortCondition ref="C1:C40"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3757E623-6D22-4D4A-BBD1-A15C4E60A30B}" name="Parameter Name"/>
@@ -684,10 +696,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -695,110 +707,110 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -811,10 +823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BCF3C8-1C6B-A245-A02F-5C0ECA1A4145}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -845,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -853,58 +865,58 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -912,23 +924,27 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -939,22 +955,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
         <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -962,200 +978,199 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
+      <c r="D20" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1166,7 +1181,7 @@
           <x14:formula1>
             <xm:f>Options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B42</xm:sqref>
+          <xm:sqref>B2:B40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Finalized sims for the proposal
</commit_message>
<xml_diff>
--- a/Varied Parameters.xlsx
+++ b/Varied Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saividyud/Documents/GitHub/NASA_25-26_Rocket_Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D90263-9D57-8342-9FD2-7873382FB059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383CFD6-DCC6-3643-B124-C276BF4C4981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{D72F03AF-D0CB-7048-A263-60968BD6DCA1}"/>
+    <workbookView xWindow="4080" yWindow="620" windowWidth="30240" windowHeight="17480" activeTab="1" xr2:uid="{D72F03AF-D0CB-7048-A263-60968BD6DCA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="2" r:id="rId1"/>
@@ -183,12 +183,6 @@
     <t>[286, 302] K</t>
   </si>
   <si>
-    <t>101325 kPa</t>
-  </si>
-  <si>
-    <t>500 kPa</t>
-  </si>
-  <si>
     <t>[0, 360) deg</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>3.4 lbs</t>
+  </si>
+  <si>
+    <t>500 Pa</t>
+  </si>
+  <si>
+    <t>101325 Pa</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BCF3C8-1C6B-A245-A02F-5C0ECA1A4145}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -885,7 +885,7 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -913,10 +913,10 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -930,15 +930,15 @@
         <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -964,13 +964,13 @@
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -984,10 +984,10 @@
         <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1001,10 +1001,10 @@
         <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1018,10 +1018,10 @@
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1035,10 +1035,10 @@
         <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1052,10 +1052,10 @@
         <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1069,10 +1069,10 @@
         <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1086,10 +1086,10 @@
         <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1103,10 +1103,10 @@
         <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1120,10 +1120,10 @@
         <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1137,7 +1137,7 @@
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -1165,7 +1165,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>